<commit_message>
Updated/Fixed Grammer in Report Files
</commit_message>
<xml_diff>
--- a/Lab1/src/Data/Lab 1 Data Files.xlsx
+++ b/Lab1/src/Data/Lab 1 Data Files.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jayso\Documents\College\CS_3353\CS-3353-Fall-2019-New\Lab1\src\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EDB62894-1755-4582-961C-574CF77A05A3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAA45109-1ADD-4E5C-86D9-3F922A607DB0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{39A37724-B21E-46B1-A5D6-9B6B53798ADF}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{39A37724-B21E-46B1-A5D6-9B6B53798ADF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -342,10 +342,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -360,20 +374,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -560,7 +560,7 @@
                   <c:v>4.43912</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>422.5</c:v>
+                  <c:v>392.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -888,6 +888,7 @@
         <c:axId val="747145080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="400"/>
           <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -1173,7 +1174,7 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.24514683217200922"/>
-          <c:y val="0.28195990026142881"/>
+          <c:y val="0.2872879050306224"/>
           <c:w val="0.6332019283426864"/>
           <c:h val="0.59974958377584786"/>
         </c:manualLayout>
@@ -1260,7 +1261,7 @@
                   <c:v>5.8619500000000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>582.61699999999996</c:v>
+                  <c:v>552.61699999999996</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1972,7 +1973,7 @@
                   <c:v>4.2822500000000003</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>415.42399999999998</c:v>
+                  <c:v>385.42399999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2305,7 +2306,7 @@
         <c:axId val="750352944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="450"/>
+          <c:max val="400"/>
           <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -2688,7 +2689,7 @@
                   <c:v>4.4008000000000003</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>420.18</c:v>
+                  <c:v>390.18</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3021,7 +3022,7 @@
         <c:axId val="750352944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="450"/>
+          <c:max val="400"/>
           <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -5575,15 +5576,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>19050</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>452438</xdr:colOff>
+      <xdr:colOff>471488</xdr:colOff>
       <xdr:row>51</xdr:row>
-      <xdr:rowOff>4763</xdr:rowOff>
+      <xdr:rowOff>42863</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5912,8 +5913,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{075DF04A-15EA-42CD-AAF6-260C4F205632}">
   <dimension ref="C2:Z29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O10" sqref="O10"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5947,25 +5948,25 @@
       </c>
     </row>
     <row r="3" spans="3:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E3" s="12" t="s">
+      <c r="E3" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="11"/>
-      <c r="G3" s="13"/>
-      <c r="J3" s="23"/>
-      <c r="L3" s="24"/>
-      <c r="N3" s="24"/>
-      <c r="P3" s="23"/>
-      <c r="Q3" s="23"/>
-      <c r="R3" s="24"/>
-      <c r="S3" s="24"/>
-      <c r="T3" s="24"/>
-      <c r="U3" s="23"/>
-      <c r="V3" s="23"/>
-      <c r="W3" s="23"/>
-      <c r="X3" s="24"/>
-      <c r="Y3" s="24"/>
-      <c r="Z3" s="24"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="23"/>
+      <c r="J3" s="17"/>
+      <c r="L3" s="18"/>
+      <c r="N3" s="18"/>
+      <c r="P3" s="17"/>
+      <c r="Q3" s="17"/>
+      <c r="R3" s="18"/>
+      <c r="S3" s="18"/>
+      <c r="T3" s="18"/>
+      <c r="U3" s="17"/>
+      <c r="V3" s="17"/>
+      <c r="W3" s="17"/>
+      <c r="X3" s="18"/>
+      <c r="Y3" s="18"/>
+      <c r="Z3" s="18"/>
     </row>
     <row r="4" spans="3:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D4" s="8" t="s">
@@ -5998,21 +5999,21 @@
         <f>G5</f>
         <v>1.18E-4</v>
       </c>
-      <c r="N4" s="23"/>
-      <c r="P4" s="23"/>
-      <c r="Q4" s="23"/>
-      <c r="R4" s="23"/>
-      <c r="S4" s="23"/>
-      <c r="T4" s="23"/>
-      <c r="U4" s="23"/>
-      <c r="V4" s="23"/>
-      <c r="W4" s="23"/>
-      <c r="X4" s="23"/>
-      <c r="Y4" s="23"/>
-      <c r="Z4" s="23"/>
+      <c r="N4" s="17"/>
+      <c r="P4" s="17"/>
+      <c r="Q4" s="17"/>
+      <c r="R4" s="17"/>
+      <c r="S4" s="17"/>
+      <c r="T4" s="17"/>
+      <c r="U4" s="17"/>
+      <c r="V4" s="17"/>
+      <c r="W4" s="17"/>
+      <c r="X4" s="17"/>
+      <c r="Y4" s="17"/>
+      <c r="Z4" s="17"/>
     </row>
     <row r="5" spans="3:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="24" t="s">
         <v>8</v>
       </c>
       <c r="D5" s="1" t="s">
@@ -6021,7 +6022,7 @@
       <c r="E5">
         <v>4.3000000000000003E-6</v>
       </c>
-      <c r="F5" s="17">
+      <c r="F5" s="11">
         <v>3.1999999999999999E-6</v>
       </c>
       <c r="G5" s="10">
@@ -6042,31 +6043,31 @@
         <f>G12</f>
         <v>9.0533000000000002E-3</v>
       </c>
-      <c r="N5" s="23"/>
-      <c r="P5" s="22"/>
-      <c r="Q5" s="23"/>
-      <c r="R5" s="23"/>
-      <c r="S5" s="23"/>
-      <c r="T5" s="23"/>
-      <c r="U5" s="23"/>
-      <c r="V5" s="22"/>
-      <c r="W5" s="23"/>
-      <c r="X5" s="23"/>
-      <c r="Y5" s="23"/>
-      <c r="Z5" s="23"/>
+      <c r="N5" s="17"/>
+      <c r="P5" s="16"/>
+      <c r="Q5" s="17"/>
+      <c r="R5" s="17"/>
+      <c r="S5" s="17"/>
+      <c r="T5" s="17"/>
+      <c r="U5" s="17"/>
+      <c r="V5" s="16"/>
+      <c r="W5" s="17"/>
+      <c r="X5" s="17"/>
+      <c r="Y5" s="17"/>
+      <c r="Z5" s="17"/>
     </row>
     <row r="6" spans="3:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C6" s="15"/>
+      <c r="C6" s="25"/>
       <c r="D6" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E6" s="4">
         <v>9.3000000000000007E-6</v>
       </c>
-      <c r="F6" s="18">
+      <c r="F6" s="12">
         <v>4.6999999999999999E-6</v>
       </c>
-      <c r="G6" s="20">
+      <c r="G6" s="14">
         <v>8.8200000000000003E-5</v>
       </c>
       <c r="J6">
@@ -6084,31 +6085,31 @@
         <f>G19</f>
         <v>0.105393</v>
       </c>
-      <c r="N6" s="23"/>
-      <c r="P6" s="22"/>
-      <c r="Q6" s="23"/>
-      <c r="R6" s="23"/>
-      <c r="S6" s="23"/>
-      <c r="T6" s="23"/>
-      <c r="U6" s="23"/>
-      <c r="V6" s="22"/>
-      <c r="W6" s="23"/>
-      <c r="X6" s="23"/>
-      <c r="Y6" s="23"/>
-      <c r="Z6" s="23"/>
+      <c r="N6" s="17"/>
+      <c r="P6" s="16"/>
+      <c r="Q6" s="17"/>
+      <c r="R6" s="17"/>
+      <c r="S6" s="17"/>
+      <c r="T6" s="17"/>
+      <c r="U6" s="17"/>
+      <c r="V6" s="16"/>
+      <c r="W6" s="17"/>
+      <c r="X6" s="17"/>
+      <c r="Y6" s="17"/>
+      <c r="Z6" s="17"/>
     </row>
     <row r="7" spans="3:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C7" s="15"/>
+      <c r="C7" s="25"/>
       <c r="D7" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E7" s="4">
         <v>3.5999999999999998E-6</v>
       </c>
-      <c r="F7" s="18">
+      <c r="F7" s="12">
         <v>1.9999999999999999E-6</v>
       </c>
-      <c r="G7" s="20">
+      <c r="G7" s="14">
         <v>5.6900000000000001E-5</v>
       </c>
       <c r="J7">
@@ -6116,7 +6117,7 @@
       </c>
       <c r="K7">
         <f>E26</f>
-        <v>422.5</v>
+        <v>392.5</v>
       </c>
       <c r="L7">
         <f>F26</f>
@@ -6126,50 +6127,50 @@
         <f>G26</f>
         <v>1.23292</v>
       </c>
-      <c r="N7" s="23"/>
-      <c r="P7" s="22"/>
-      <c r="Q7" s="23"/>
-      <c r="R7" s="23"/>
-      <c r="S7" s="23"/>
-      <c r="T7" s="23"/>
-      <c r="U7" s="23"/>
-      <c r="V7" s="22"/>
-      <c r="W7" s="23"/>
-      <c r="X7" s="23"/>
-      <c r="Y7" s="23"/>
-      <c r="Z7" s="23"/>
+      <c r="N7" s="17"/>
+      <c r="P7" s="16"/>
+      <c r="Q7" s="17"/>
+      <c r="R7" s="17"/>
+      <c r="S7" s="17"/>
+      <c r="T7" s="17"/>
+      <c r="U7" s="17"/>
+      <c r="V7" s="16"/>
+      <c r="W7" s="17"/>
+      <c r="X7" s="17"/>
+      <c r="Y7" s="17"/>
+      <c r="Z7" s="17"/>
     </row>
     <row r="8" spans="3:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C8" s="16"/>
+      <c r="C8" s="26"/>
       <c r="D8" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E8" s="6">
         <v>3.7000000000000002E-6</v>
       </c>
-      <c r="F8" s="19">
+      <c r="F8" s="13">
         <v>2.5000000000000002E-6</v>
       </c>
-      <c r="G8" s="21">
+      <c r="G8" s="15">
         <v>5.6199999999999997E-5</v>
       </c>
-      <c r="J8" s="22"/>
-      <c r="K8" s="23"/>
-      <c r="L8" s="23"/>
-      <c r="M8" s="23"/>
-      <c r="N8" s="23"/>
-      <c r="O8" s="23"/>
-      <c r="P8" s="22"/>
-      <c r="Q8" s="23"/>
-      <c r="R8" s="23"/>
-      <c r="S8" s="23"/>
-      <c r="T8" s="23"/>
-      <c r="U8" s="23"/>
-      <c r="V8" s="22"/>
-      <c r="W8" s="23"/>
-      <c r="X8" s="23"/>
-      <c r="Y8" s="23"/>
-      <c r="Z8" s="23"/>
+      <c r="J8" s="16"/>
+      <c r="K8" s="17"/>
+      <c r="L8" s="17"/>
+      <c r="M8" s="17"/>
+      <c r="N8" s="17"/>
+      <c r="O8" s="17"/>
+      <c r="P8" s="16"/>
+      <c r="Q8" s="17"/>
+      <c r="R8" s="17"/>
+      <c r="S8" s="17"/>
+      <c r="T8" s="17"/>
+      <c r="U8" s="17"/>
+      <c r="V8" s="16"/>
+      <c r="W8" s="17"/>
+      <c r="X8" s="17"/>
+      <c r="Y8" s="17"/>
+      <c r="Z8" s="17"/>
     </row>
     <row r="9" spans="3:26" x14ac:dyDescent="0.25">
       <c r="I9" t="s">
@@ -6178,66 +6179,66 @@
       <c r="J9">
         <v>10</v>
       </c>
-      <c r="K9" s="26">
+      <c r="K9" s="20">
         <f>E6</f>
         <v>9.3000000000000007E-6</v>
       </c>
-      <c r="L9" s="26">
+      <c r="L9" s="20">
         <f>F6</f>
         <v>4.6999999999999999E-6</v>
       </c>
-      <c r="M9" s="26">
+      <c r="M9" s="20">
         <f>G6</f>
         <v>8.8200000000000003E-5</v>
       </c>
-      <c r="N9" s="25"/>
-      <c r="O9" s="25"/>
-      <c r="P9" s="25"/>
-      <c r="Q9" s="25"/>
-      <c r="R9" s="25"/>
-      <c r="S9" s="25"/>
-      <c r="T9" s="25"/>
-      <c r="U9" s="25"/>
-      <c r="V9" s="25"/>
-      <c r="W9" s="25"/>
-      <c r="X9" s="25"/>
-      <c r="Y9" s="25"/>
-      <c r="Z9" s="25"/>
+      <c r="N9" s="19"/>
+      <c r="O9" s="19"/>
+      <c r="P9" s="19"/>
+      <c r="Q9" s="19"/>
+      <c r="R9" s="19"/>
+      <c r="S9" s="19"/>
+      <c r="T9" s="19"/>
+      <c r="U9" s="19"/>
+      <c r="V9" s="19"/>
+      <c r="W9" s="19"/>
+      <c r="X9" s="19"/>
+      <c r="Y9" s="19"/>
+      <c r="Z9" s="19"/>
     </row>
     <row r="10" spans="3:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E10" s="12" t="s">
+      <c r="E10" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="F10" s="11"/>
-      <c r="G10" s="13"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="23"/>
       <c r="J10">
         <v>1000</v>
       </c>
-      <c r="K10" s="23">
+      <c r="K10" s="17">
         <f>E13</f>
         <v>5.6708399999999999E-2</v>
       </c>
-      <c r="L10" s="23">
+      <c r="L10" s="17">
         <f>F13</f>
         <v>3.8680800000000001E-2</v>
       </c>
-      <c r="M10" s="23">
+      <c r="M10" s="17">
         <f>G13</f>
         <v>1.0019200000000001E-2</v>
       </c>
-      <c r="N10" s="25"/>
-      <c r="O10" s="25"/>
-      <c r="P10" s="25"/>
-      <c r="Q10" s="25"/>
-      <c r="R10" s="25"/>
-      <c r="S10" s="25"/>
-      <c r="T10" s="25"/>
-      <c r="U10" s="25"/>
-      <c r="V10" s="25"/>
-      <c r="W10" s="25"/>
-      <c r="X10" s="25"/>
-      <c r="Y10" s="25"/>
-      <c r="Z10" s="25"/>
+      <c r="N10" s="19"/>
+      <c r="O10" s="19"/>
+      <c r="P10" s="19"/>
+      <c r="Q10" s="19"/>
+      <c r="R10" s="19"/>
+      <c r="S10" s="19"/>
+      <c r="T10" s="19"/>
+      <c r="U10" s="19"/>
+      <c r="V10" s="19"/>
+      <c r="W10" s="19"/>
+      <c r="X10" s="19"/>
+      <c r="Y10" s="19"/>
+      <c r="Z10" s="19"/>
     </row>
     <row r="11" spans="3:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D11" s="8" t="s">
@@ -6255,34 +6256,34 @@
       <c r="J11">
         <v>10000</v>
       </c>
-      <c r="K11" s="23">
+      <c r="K11" s="17">
         <f>E20</f>
         <v>5.8619500000000002</v>
       </c>
-      <c r="L11" s="23">
+      <c r="L11" s="17">
         <f>F20</f>
         <v>3.5114399999999999</v>
       </c>
-      <c r="M11" s="23">
+      <c r="M11" s="17">
         <f>G20</f>
         <v>0.105105</v>
       </c>
-      <c r="N11" s="25"/>
-      <c r="O11" s="25"/>
-      <c r="P11" s="25"/>
-      <c r="Q11" s="25"/>
-      <c r="R11" s="25"/>
-      <c r="S11" s="25"/>
-      <c r="T11" s="25"/>
-      <c r="U11" s="25"/>
-      <c r="V11" s="25"/>
-      <c r="W11" s="25"/>
-      <c r="X11" s="25"/>
-      <c r="Y11" s="25"/>
-      <c r="Z11" s="25"/>
+      <c r="N11" s="19"/>
+      <c r="O11" s="19"/>
+      <c r="P11" s="19"/>
+      <c r="Q11" s="19"/>
+      <c r="R11" s="19"/>
+      <c r="S11" s="19"/>
+      <c r="T11" s="19"/>
+      <c r="U11" s="19"/>
+      <c r="V11" s="19"/>
+      <c r="W11" s="19"/>
+      <c r="X11" s="19"/>
+      <c r="Y11" s="19"/>
+      <c r="Z11" s="19"/>
     </row>
     <row r="12" spans="3:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C12" s="14" t="s">
+      <c r="C12" s="24" t="s">
         <v>8</v>
       </c>
       <c r="D12" s="1" t="s">
@@ -6300,34 +6301,34 @@
       <c r="J12">
         <v>100000</v>
       </c>
-      <c r="K12" s="23">
+      <c r="K12" s="17">
         <f>E27</f>
-        <v>582.61699999999996</v>
-      </c>
-      <c r="L12" s="23">
+        <v>552.61699999999996</v>
+      </c>
+      <c r="L12" s="17">
         <f>F27</f>
         <v>326.42099999999999</v>
       </c>
-      <c r="M12" s="23">
+      <c r="M12" s="17">
         <f>G27</f>
         <v>1.1498900000000001</v>
       </c>
-      <c r="N12" s="25"/>
-      <c r="O12" s="25"/>
-      <c r="P12" s="25"/>
-      <c r="Q12" s="25"/>
-      <c r="R12" s="25"/>
-      <c r="S12" s="25"/>
-      <c r="T12" s="25"/>
-      <c r="U12" s="25"/>
-      <c r="V12" s="25"/>
-      <c r="W12" s="25"/>
-      <c r="X12" s="25"/>
-      <c r="Y12" s="25"/>
-      <c r="Z12" s="25"/>
+      <c r="N12" s="19"/>
+      <c r="O12" s="19"/>
+      <c r="P12" s="19"/>
+      <c r="Q12" s="19"/>
+      <c r="R12" s="19"/>
+      <c r="S12" s="19"/>
+      <c r="T12" s="19"/>
+      <c r="U12" s="19"/>
+      <c r="V12" s="19"/>
+      <c r="W12" s="19"/>
+      <c r="X12" s="19"/>
+      <c r="Y12" s="19"/>
+      <c r="Z12" s="19"/>
     </row>
     <row r="13" spans="3:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="15"/>
+      <c r="C13" s="25"/>
       <c r="D13" s="1" t="s">
         <v>1</v>
       </c>
@@ -6342,7 +6343,7 @@
       </c>
     </row>
     <row r="14" spans="3:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C14" s="15"/>
+      <c r="C14" s="25"/>
       <c r="D14" s="1" t="s">
         <v>2</v>
       </c>
@@ -6361,21 +6362,21 @@
       <c r="J14">
         <v>10</v>
       </c>
-      <c r="K14" s="24">
+      <c r="K14" s="18">
         <f>E7</f>
         <v>3.5999999999999998E-6</v>
       </c>
-      <c r="L14" s="24">
+      <c r="L14" s="18">
         <f>F7</f>
         <v>1.9999999999999999E-6</v>
       </c>
-      <c r="M14" s="24">
+      <c r="M14" s="18">
         <f>G7</f>
         <v>5.6900000000000001E-5</v>
       </c>
     </row>
     <row r="15" spans="3:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C15" s="16"/>
+      <c r="C15" s="26"/>
       <c r="D15" s="1" t="s">
         <v>3</v>
       </c>
@@ -6391,15 +6392,15 @@
       <c r="J15">
         <v>1000</v>
       </c>
-      <c r="K15" s="23">
+      <c r="K15" s="17">
         <f>E14</f>
         <v>4.7468499999999997E-2</v>
       </c>
-      <c r="L15" s="23">
+      <c r="L15" s="17">
         <f>F14</f>
         <v>1.55528E-2</v>
       </c>
-      <c r="M15" s="23">
+      <c r="M15" s="17">
         <f>G14</f>
         <v>8.6309999999999998E-3</v>
       </c>
@@ -6408,37 +6409,37 @@
       <c r="J16">
         <v>10000</v>
       </c>
-      <c r="K16" s="23">
+      <c r="K16" s="17">
         <f>E21</f>
         <v>4.2822500000000003</v>
       </c>
-      <c r="L16" s="23">
+      <c r="L16" s="17">
         <f>F21</f>
         <v>1.6527099999999999</v>
       </c>
-      <c r="M16" s="23">
+      <c r="M16" s="17">
         <f>G21</f>
         <v>0.10745499999999999</v>
       </c>
     </row>
     <row r="17" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E17" s="12" t="s">
+      <c r="E17" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="F17" s="11"/>
-      <c r="G17" s="13"/>
+      <c r="F17" s="22"/>
+      <c r="G17" s="23"/>
       <c r="J17">
         <v>100000</v>
       </c>
-      <c r="K17" s="23">
+      <c r="K17" s="17">
         <f>E28</f>
-        <v>415.42399999999998</v>
-      </c>
-      <c r="L17" s="23">
+        <v>385.42399999999998</v>
+      </c>
+      <c r="L17" s="17">
         <f>F28</f>
         <v>162.82300000000001</v>
       </c>
-      <c r="M17" s="23">
+      <c r="M17" s="17">
         <f>G28</f>
         <v>1.19895</v>
       </c>
@@ -6458,7 +6459,7 @@
       </c>
     </row>
     <row r="19" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C19" s="14" t="s">
+      <c r="C19" s="24" t="s">
         <v>8</v>
       </c>
       <c r="D19" s="1" t="s">
@@ -6479,21 +6480,21 @@
       <c r="J19">
         <v>10</v>
       </c>
-      <c r="K19" s="23">
+      <c r="K19" s="17">
         <f>E8</f>
         <v>3.7000000000000002E-6</v>
       </c>
-      <c r="L19" s="23">
+      <c r="L19" s="17">
         <f>F8</f>
         <v>2.5000000000000002E-6</v>
       </c>
-      <c r="M19" s="23">
+      <c r="M19" s="17">
         <f>G8</f>
         <v>5.6199999999999997E-5</v>
       </c>
     </row>
     <row r="20" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C20" s="15"/>
+      <c r="C20" s="25"/>
       <c r="D20" s="1" t="s">
         <v>1</v>
       </c>
@@ -6509,21 +6510,21 @@
       <c r="J20">
         <v>1000</v>
       </c>
-      <c r="K20" s="23">
+      <c r="K20" s="17">
         <f>E15</f>
         <v>4.3419699999999999E-2</v>
       </c>
-      <c r="L20" s="23">
+      <c r="L20" s="17">
         <f>F15</f>
         <v>1.50794E-2</v>
       </c>
-      <c r="M20" s="23">
+      <c r="M20" s="17">
         <f>G15</f>
         <v>1.15563E-2</v>
       </c>
     </row>
     <row r="21" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C21" s="15"/>
+      <c r="C21" s="25"/>
       <c r="D21" s="1" t="s">
         <v>2</v>
       </c>
@@ -6539,21 +6540,21 @@
       <c r="J21">
         <v>10000</v>
       </c>
-      <c r="K21" s="23">
+      <c r="K21" s="17">
         <f>E22</f>
         <v>4.4008000000000003</v>
       </c>
-      <c r="L21" s="23">
+      <c r="L21" s="17">
         <f>F22</f>
         <v>1.4886699999999999</v>
       </c>
-      <c r="M21" s="23">
+      <c r="M21" s="17">
         <f>G22</f>
         <v>0.110787</v>
       </c>
     </row>
     <row r="22" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C22" s="16"/>
+      <c r="C22" s="26"/>
       <c r="D22" s="1" t="s">
         <v>3</v>
       </c>
@@ -6569,25 +6570,25 @@
       <c r="J22">
         <v>100000</v>
       </c>
-      <c r="K22" s="23">
+      <c r="K22" s="17">
         <f>E29</f>
-        <v>420.18</v>
-      </c>
-      <c r="L22" s="23">
+        <v>390.18</v>
+      </c>
+      <c r="L22" s="17">
         <f>F29</f>
         <v>152.00200000000001</v>
       </c>
-      <c r="M22" s="23">
+      <c r="M22" s="17">
         <f>G29</f>
         <v>1.15218</v>
       </c>
     </row>
     <row r="24" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E24" s="12" t="s">
+      <c r="E24" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="F24" s="11"/>
-      <c r="G24" s="13"/>
+      <c r="F24" s="22"/>
+      <c r="G24" s="23"/>
     </row>
     <row r="25" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D25" s="8" t="s">
@@ -6604,14 +6605,14 @@
       </c>
     </row>
     <row r="26" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C26" s="14" t="s">
+      <c r="C26" s="24" t="s">
         <v>8</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>0</v>
       </c>
       <c r="E26" s="2">
-        <v>422.5</v>
+        <v>392.5</v>
       </c>
       <c r="F26" s="5">
         <v>174.68</v>
@@ -6621,12 +6622,12 @@
       </c>
     </row>
     <row r="27" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C27" s="15"/>
+      <c r="C27" s="25"/>
       <c r="D27" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E27" s="4">
-        <v>582.61699999999996</v>
+        <v>552.61699999999996</v>
       </c>
       <c r="F27" s="3">
         <v>326.42099999999999</v>
@@ -6636,12 +6637,12 @@
       </c>
     </row>
     <row r="28" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C28" s="15"/>
+      <c r="C28" s="25"/>
       <c r="D28" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E28" s="4">
-        <v>415.42399999999998</v>
+        <v>385.42399999999998</v>
       </c>
       <c r="F28" s="3">
         <v>162.82300000000001</v>
@@ -6651,12 +6652,12 @@
       </c>
     </row>
     <row r="29" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C29" s="16"/>
+      <c r="C29" s="26"/>
       <c r="D29" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E29" s="6">
-        <v>420.18</v>
+        <v>390.18</v>
       </c>
       <c r="F29" s="7">
         <v>152.00200000000001</v>
@@ -6667,14 +6668,14 @@
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="C5:C8"/>
     <mergeCell ref="E24:G24"/>
     <mergeCell ref="C26:C29"/>
     <mergeCell ref="E10:G10"/>
     <mergeCell ref="C12:C15"/>
     <mergeCell ref="E17:G17"/>
     <mergeCell ref="C19:C22"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="C5:C8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>